<commit_message>
#1 Csv done for now
</commit_message>
<xml_diff>
--- a/TestSystem/resources/Dataen.xlsx
+++ b/TestSystem/resources/Dataen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Not David Bowie\Desktop\3i_test_nummer1-master\TestSystem\TestSystem\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E27400-C9AE-46C5-A15E-345EB066A919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{423ABE68-62C6-4C71-85B3-D9AB93B8DB34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="2160" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="121">
   <si>
     <t>Foto</t>
   </si>
@@ -709,6 +709,9 @@
   </si>
   <si>
     <t>Vald435P</t>
+  </si>
+  <si>
+    <t>Score</t>
   </si>
 </sst>
 </file>
@@ -1053,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,7 +1072,7 @@
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1094,8 +1097,11 @@
       <c r="H1" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -1117,7 +1123,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="3" t="s">
         <v>6</v>
@@ -1139,7 +1145,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -1163,7 +1169,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>13</v>
@@ -1187,7 +1193,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>13</v>
@@ -1211,7 +1217,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
         <v>13</v>
@@ -1235,7 +1241,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>13</v>
@@ -1259,7 +1265,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
         <v>13</v>
@@ -1283,7 +1289,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
         <v>13</v>
@@ -1307,7 +1313,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
         <v>13</v>
@@ -1331,7 +1337,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
         <v>13</v>
@@ -1355,7 +1361,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
         <v>13</v>
@@ -1379,7 +1385,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
         <v>13</v>
@@ -1403,7 +1409,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
         <v>13</v>
@@ -1427,7 +1433,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
         <v>13</v>

</xml_diff>